<commit_message>
Column header as the key
</commit_message>
<xml_diff>
--- a/data/datafile-extracted.xlsx
+++ b/data/datafile-extracted.xlsx
@@ -14,37 +14,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
-    <t>Usage</t>
+    <t>usage</t>
   </si>
   <si>
-    <t>Viewport Width</t>
+    <t>viewportWidth</t>
   </si>
   <si>
-    <t>Pixel Ratio</t>
+    <t>pixelRatio</t>
   </si>
   <si>
-    <t>Img Width</t>
+    <t>imgWidth</t>
   </si>
   <si>
-    <t>Img V W</t>
+    <t>imgVW</t>
   </si>
   <si>
-    <t>Ideal Intrinsic Width</t>
+    <t>idealIntrinsicWidth</t>
   </si>
   <si>
-    <t>Chosen Intrinsic Width</t>
+    <t>chosenIntrinsicWidth</t>
   </si>
   <si>
-    <t>Rendered Fidelity</t>
+    <t>renderedFidelity</t>
   </si>
   <si>
-    <t>Rendered To Ideal Fidelity Ratio</t>
+    <t>renderedToIdealFidelityRatio</t>
   </si>
   <si>
-    <t>Evaluation</t>
+    <t>evaluation</t>
   </si>
   <si>
-    <t>Waste</t>
+    <t>waste</t>
   </si>
 </sst>
 </file>
@@ -433,14 +433,14 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23" style="3" customWidth="1"/>
-    <col min="8" max="8" width="18" style="4" customWidth="1"/>
-    <col min="9" max="9" width="33" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17" style="4" customWidth="1"/>
+    <col min="9" max="9" width="29" style="4" customWidth="1"/>
     <col min="10" max="10" width="16" style="2" customWidth="1"/>
     <col min="11" max="11" width="16" style="1" customWidth="1"/>
   </cols>
@@ -1052,14 +1052,14 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23" style="3" customWidth="1"/>
-    <col min="8" max="8" width="18" style="4" customWidth="1"/>
-    <col min="9" max="9" width="33" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17" style="4" customWidth="1"/>
+    <col min="9" max="9" width="29" style="4" customWidth="1"/>
     <col min="10" max="10" width="16" style="2" customWidth="1"/>
     <col min="11" max="11" width="16" style="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Fixed extraction and algorthm to generate uncapped
</commit_message>
<xml_diff>
--- a/data/datafile-extracted.xlsx
+++ b/data/datafile-extracted.xlsx
@@ -494,7 +494,7 @@
         <v>172</v>
       </c>
       <c r="E2" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2">
         <v>344</v>
@@ -529,7 +529,7 @@
         <v>190</v>
       </c>
       <c r="E3" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2">
         <v>380</v>
@@ -564,7 +564,7 @@
         <v>179</v>
       </c>
       <c r="E4" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2">
         <v>358</v>
@@ -599,7 +599,7 @@
         <v>172</v>
       </c>
       <c r="E5" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2">
         <v>344</v>
@@ -634,7 +634,7 @@
         <v>190</v>
       </c>
       <c r="E6" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F6" s="2">
         <v>380</v>
@@ -669,7 +669,7 @@
         <v>165</v>
       </c>
       <c r="E7" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2">
         <v>330</v>
@@ -704,7 +704,7 @@
         <v>196</v>
       </c>
       <c r="E8" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2">
         <v>392</v>
@@ -739,7 +739,7 @@
         <v>450</v>
       </c>
       <c r="E9" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="2">
         <v>450</v>
@@ -774,7 +774,7 @@
         <v>189</v>
       </c>
       <c r="E10" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2">
         <v>378</v>
@@ -809,7 +809,7 @@
         <v>339</v>
       </c>
       <c r="E11" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2">
         <v>678</v>
@@ -844,7 +844,7 @@
         <v>321</v>
       </c>
       <c r="E12" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2">
         <v>321</v>
@@ -879,7 +879,7 @@
         <v>165</v>
       </c>
       <c r="E13" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F13" s="2">
         <v>330</v>
@@ -914,7 +914,7 @@
         <v>352</v>
       </c>
       <c r="E14" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F14" s="2">
         <v>704</v>
@@ -949,7 +949,7 @@
         <v>180</v>
       </c>
       <c r="E15" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F15" s="2">
         <v>360</v>
@@ -984,7 +984,7 @@
         <v>361</v>
       </c>
       <c r="E16" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2">
         <v>451</v>
@@ -1019,7 +1019,7 @@
         <v>147</v>
       </c>
       <c r="E17" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F17" s="2">
         <v>294</v>
@@ -1113,7 +1113,7 @@
         <v>172</v>
       </c>
       <c r="E2" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2">
         <v>516</v>
@@ -1148,7 +1148,7 @@
         <v>190</v>
       </c>
       <c r="E3" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2">
         <v>380</v>
@@ -1183,7 +1183,7 @@
         <v>179</v>
       </c>
       <c r="E4" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2">
         <v>537</v>
@@ -1218,7 +1218,7 @@
         <v>172</v>
       </c>
       <c r="E5" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2">
         <v>344</v>
@@ -1253,7 +1253,7 @@
         <v>190</v>
       </c>
       <c r="E6" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F6" s="2">
         <v>570</v>
@@ -1288,7 +1288,7 @@
         <v>165</v>
       </c>
       <c r="E7" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2">
         <v>495</v>
@@ -1323,7 +1323,7 @@
         <v>196</v>
       </c>
       <c r="E8" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2">
         <v>588</v>
@@ -1358,7 +1358,7 @@
         <v>780</v>
       </c>
       <c r="E9" s="2">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2">
         <v>780</v>
@@ -1393,7 +1393,7 @@
         <v>189</v>
       </c>
       <c r="E10" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2">
         <v>497</v>
@@ -1428,7 +1428,7 @@
         <v>551</v>
       </c>
       <c r="E11" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="2">
         <v>1102</v>
@@ -1463,7 +1463,7 @@
         <v>522</v>
       </c>
       <c r="E12" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" s="2">
         <v>522</v>
@@ -1498,7 +1498,7 @@
         <v>165</v>
       </c>
       <c r="E13" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F13" s="2">
         <v>330</v>
@@ -1533,7 +1533,7 @@
         <v>352</v>
       </c>
       <c r="E14" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F14" s="2">
         <v>704</v>
@@ -1568,7 +1568,7 @@
         <v>180</v>
       </c>
       <c r="E15" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F15" s="2">
         <v>495</v>
@@ -1603,7 +1603,7 @@
         <v>587</v>
       </c>
       <c r="E16" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16" s="2">
         <v>734</v>
@@ -1638,7 +1638,7 @@
         <v>147</v>
       </c>
       <c r="E17" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F17" s="2">
         <v>294</v>

</xml_diff>

<commit_message>
Added conditional formatting based on evaluation
</commit_message>
<xml_diff>
--- a/data/datafile-extracted.xlsx
+++ b/data/datafile-extracted.xlsx
@@ -1,12 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10215"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518BEDBA-DFC9-8E4B-9C21-205C07A29D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="listing" state="visible" r:id="rId4"/>
+    <sheet name="listing" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -49,30 +65,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF1CC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -84,8 +98,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -97,13 +115,48 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD4EDD2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC0504D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF99D07A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -437,9 +490,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -453,7 +511,7 @@
     <col min="11" max="11" width="16" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,9 +546,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0.139</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -512,20 +570,24 @@
       </c>
       <c r="H2" s="3">
         <f t="shared" ref="H2:H17" si="0">G2/D2</f>
+        <v>2.2093023255813953</v>
       </c>
       <c r="I2" s="3">
         <f t="shared" ref="I2:I17" si="1">H2/MIN(2, C2)</f>
-      </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J17" si="2">_xlfn.IFS(I2&lt;0.9, "POOR! (--)", I2&lt;1, "(-)", I2=1, "OK", I2&gt;1.2, "BIG (++)", I2&gt;1, "(+)")</f>
+        <v>1.1046511627906976</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J17" si="2">_xlfn.IFS(I2&lt;0.9, "POOR (--)", I2&lt;1, "(-)", I2=1, "GOOD!", I2&gt;1.2, "BIG (++)", I2&gt;1, "(+)")</f>
+        <v>(+)</v>
       </c>
       <c r="K2" s="1">
         <f t="shared" ref="K2:K17" si="3">(I2-1)*A2</f>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.4546511627906973E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>0.134</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="B3">
         <v>414</v>
@@ -547,20 +609,24 @@
       </c>
       <c r="H3" s="3">
         <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J3">
-        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="2"/>
+        <v>GOOD!</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>0.095</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="B4">
         <v>390</v>
@@ -582,20 +648,24 @@
       </c>
       <c r="H4" s="3">
         <f t="shared" si="0"/>
+        <v>2.1229050279329611</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
+        <v>1.0614525139664805</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="2"/>
+        <v>(+)</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.8379888268156521E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>0.086</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="B5">
         <v>375</v>
@@ -617,20 +687,24 @@
       </c>
       <c r="H5" s="3">
         <f t="shared" si="0"/>
+        <v>2.2093023255813953</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
+        <v>1.1046511627906976</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="2"/>
+        <v>(+)</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.9999999999999959E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>0.083</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="B6">
         <v>414</v>
@@ -652,20 +726,24 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="2"/>
+        <v>GOOD!</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="B7">
         <v>360</v>
@@ -687,20 +765,24 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
+        <v>2.3030303030303032</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
+        <v>1.1515151515151516</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="2"/>
+        <v>(+)</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.2424242424242482E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>0.052000000000000005</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="B8">
         <v>428</v>
@@ -722,20 +804,24 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" si="0"/>
+        <v>1.9387755102040816</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
+        <v>0.96938775510204078</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="2"/>
+        <v>(-)</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-1.5918367346938794E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>0.040999999999999995</v>
+        <v>4.0999999999999995E-2</v>
       </c>
       <c r="B9">
         <v>1920</v>
@@ -753,24 +839,28 @@
         <v>450</v>
       </c>
       <c r="G9" s="2">
-        <v>380</v>
+        <v>450</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="2"/>
+        <v>GOOD!</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>0.037000000000000005</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="B10">
         <v>412</v>
@@ -792,20 +882,24 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
+        <v>2.0105820105820107</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
+        <v>1.0052910052910053</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="2"/>
+        <v>(+)</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.9576719576719785E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
       <c r="B11">
         <v>1440</v>
@@ -823,24 +917,28 @@
         <v>678</v>
       </c>
       <c r="G11" s="2">
-        <v>380</v>
+        <v>678</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="2"/>
+        <v>GOOD!</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>0.018000000000000002</v>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="B12">
         <v>1366</v>
@@ -862,20 +960,24 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" si="0"/>
+        <v>1.1838006230529594</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
+        <v>1.1838006230529594</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="2"/>
+        <v>(+)</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.3084112149532698E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="B13">
         <v>360</v>
@@ -897,20 +999,24 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" si="0"/>
+        <v>2.3030303030303032</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
+        <v>1.1515151515151516</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="2"/>
+        <v>(+)</v>
       </c>
       <c r="K13" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.4242424242424255E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="B14">
         <v>768</v>
@@ -928,24 +1034,28 @@
         <v>704</v>
       </c>
       <c r="G14" s="2">
-        <v>380</v>
+        <v>704</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J14">
-        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="2"/>
+        <v>GOOD!</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>0.013999999999999999</v>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="B15">
         <v>393</v>
@@ -967,20 +1077,24 @@
       </c>
       <c r="H15" s="3">
         <f t="shared" si="0"/>
+        <v>2.1111111111111112</v>
       </c>
       <c r="I15" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
+        <v>1.0555555555555556</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="2"/>
+        <v>(+)</v>
       </c>
       <c r="K15" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.7777777777777806E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>0.011000000000000001</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="B16">
         <v>1536</v>
@@ -998,24 +1112,28 @@
         <v>451</v>
       </c>
       <c r="G16" s="2">
-        <v>380</v>
+        <v>450</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="0"/>
+        <v>1.2465373961218837</v>
       </c>
       <c r="I16" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
+        <v>0.99722991689750695</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="2"/>
+        <v>(-)</v>
       </c>
       <c r="K16" s="1">
         <f t="shared" si="3"/>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.0470914127423535E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="B17">
         <v>320</v>
@@ -1037,19 +1155,37 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" si="0"/>
+        <v>2.5850340136054424</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
+        <v>1.2925170068027212</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="K17" s="1">
         <f t="shared" si="3"/>
+        <v>2.3401360544217696E-3</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:G17">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>J2="GOOD!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>J2="POOR (--)"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>J2="BIG (++)"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>OR(J2="(+)",J2="(-)")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Managed to get image intrinsic sizes with probe
</commit_message>
<xml_diff>
--- a/data/datafile-extracted.xlsx
+++ b/data/datafile-extracted.xlsx
@@ -1,33 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10215"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518BEDBA-DFC9-8E4B-9C21-205C07A29D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="listing" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="home" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>usage</t>
   </si>
@@ -42,6 +26,9 @@
   </si>
   <si>
     <t>imgVW</t>
+  </si>
+  <si>
+    <t>currentIntrinsicWidth</t>
   </si>
   <si>
     <t>idealIntrinsicWidth</t>
@@ -65,20 +52,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,12 +82,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -125,7 +105,17 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFD4EDD2"/>
+          <bgColor rgb="FF99D07A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC0504D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -140,19 +130,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFC0504D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF99D07A"/>
+          <bgColor rgb="FFD4EDD2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -490,28 +470,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L17"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17" style="3" customWidth="1"/>
-    <col min="9" max="9" width="29" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="16" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="21" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17" style="3" customWidth="1"/>
+    <col min="10" max="10" width="29" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="6" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,25 +506,28 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.13900000000000001</v>
+        <v>0.139</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -557,37 +536,34 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>172</v>
+        <v>335</v>
       </c>
       <c r="E2">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="F2">
-        <v>344</v>
-      </c>
-      <c r="G2" s="2">
-        <v>380</v>
-      </c>
-      <c r="H2" s="3">
+        <v>1024</v>
+      </c>
+      <c r="G2">
+        <v>670</v>
+      </c>
+      <c r="H2" s="2">
         <f t="shared" ref="H2:H17" si="0">G2/D2</f>
-        <v>2.2093023255813953</v>
       </c>
       <c r="I2" s="3">
         <f t="shared" ref="I2:I17" si="1">H2/MIN(2, C2)</f>
-        <v>1.1046511627906976</v>
-      </c>
-      <c r="J2" t="str">
+      </c>
+      <c r="J2" s="3">
         <f t="shared" ref="J2:J17" si="2">_xlfn.IFS(I2&lt;0.9, "POOR (--)", I2&lt;1, "(-)", I2=1, "GOOD!", I2&gt;1.2, "BIG (++)", I2&gt;1, "(+)")</f>
-        <v>(+)</v>
-      </c>
-      <c r="K2" s="1">
+      </c>
+      <c r="K2">
         <f t="shared" ref="K2:K17" si="3">(I2-1)*A2</f>
-        <v>1.4546511627906973E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.13400000000000001</v>
+        <v>0.134</v>
       </c>
       <c r="B3">
         <v>414</v>
@@ -596,37 +572,34 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>190</v>
+        <v>374</v>
       </c>
       <c r="E3">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F3">
-        <v>380</v>
-      </c>
-      <c r="G3" s="2">
-        <v>380</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1024</v>
+      </c>
+      <c r="G3">
+        <v>748</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I3" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J3" t="str">
-        <f t="shared" si="2"/>
-        <v>GOOD!</v>
-      </c>
-      <c r="K3" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K3">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>0.095</v>
       </c>
       <c r="B4">
         <v>390</v>
@@ -635,37 +608,34 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>179</v>
+        <v>350</v>
       </c>
       <c r="E4">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="F4">
-        <v>358</v>
-      </c>
-      <c r="G4" s="2">
-        <v>380</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="0"/>
-        <v>2.1229050279329611</v>
+        <v>1024</v>
+      </c>
+      <c r="G4">
+        <v>700</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="1"/>
-        <v>1.0614525139664805</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
-      </c>
-      <c r="K4" s="1">
-        <f t="shared" si="3"/>
-        <v>5.8379888268156521E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>0.086</v>
       </c>
       <c r="B5">
         <v>375</v>
@@ -674,37 +644,34 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>172</v>
+        <v>335</v>
       </c>
       <c r="E5">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="F5">
-        <v>344</v>
-      </c>
-      <c r="G5" s="2">
-        <v>380</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="0"/>
-        <v>2.2093023255813953</v>
+        <v>1024</v>
+      </c>
+      <c r="G5">
+        <v>670</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I5" s="3">
         <f t="shared" si="1"/>
-        <v>1.1046511627906976</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="3"/>
-        <v>8.9999999999999959E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>0.083</v>
       </c>
       <c r="B6">
         <v>414</v>
@@ -713,37 +680,34 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>190</v>
+        <v>374</v>
       </c>
       <c r="E6">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F6">
-        <v>380</v>
-      </c>
-      <c r="G6" s="2">
-        <v>380</v>
-      </c>
-      <c r="H6" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1024</v>
+      </c>
+      <c r="G6">
+        <v>748</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I6" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="2"/>
-        <v>GOOD!</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>0.061</v>
       </c>
       <c r="B7">
         <v>360</v>
@@ -752,37 +716,34 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="E7">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="F7">
-        <v>330</v>
-      </c>
-      <c r="G7" s="2">
-        <v>380</v>
-      </c>
-      <c r="H7" s="3">
-        <f t="shared" si="0"/>
-        <v>2.3030303030303032</v>
+        <v>1024</v>
+      </c>
+      <c r="G7">
+        <v>640</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>1.1515151515151516</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="3"/>
-        <v>9.2424242424242482E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5.2000000000000005E-2</v>
+        <v>0.052000000000000005</v>
       </c>
       <c r="B8">
         <v>428</v>
@@ -791,37 +752,34 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <v>196</v>
+        <v>388</v>
       </c>
       <c r="E8">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F8">
-        <v>392</v>
-      </c>
-      <c r="G8" s="2">
-        <v>380</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" si="0"/>
-        <v>1.9387755102040816</v>
+        <v>1024</v>
+      </c>
+      <c r="G8">
+        <v>776</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="1"/>
-        <v>0.96938775510204078</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="2"/>
-        <v>(-)</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="3"/>
-        <v>-1.5918367346938794E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>4.0999999999999995E-2</v>
+        <v>0.040999999999999995</v>
       </c>
       <c r="B9">
         <v>1920</v>
@@ -830,37 +788,34 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>450</v>
+        <v>1680</v>
       </c>
       <c r="E9">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="F9">
-        <v>450</v>
-      </c>
-      <c r="G9" s="2">
-        <v>450</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1680</v>
+      </c>
+      <c r="G9">
+        <v>1680</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="2"/>
-        <v>GOOD!</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>3.7000000000000005E-2</v>
+        <v>0.037000000000000005</v>
       </c>
       <c r="B10">
         <v>412</v>
@@ -869,37 +824,34 @@
         <v>2.63</v>
       </c>
       <c r="D10">
-        <v>189</v>
+        <v>372</v>
       </c>
       <c r="E10">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F10">
-        <v>378</v>
-      </c>
-      <c r="G10" s="2">
-        <v>380</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
-        <v>2.0105820105820107</v>
+        <v>1024</v>
+      </c>
+      <c r="G10">
+        <v>744</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="1"/>
-        <v>1.0052910052910053</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="3"/>
-        <v>1.9576719576719785E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.3E-2</v>
+        <v>0.023</v>
       </c>
       <c r="B11">
         <v>1440</v>
@@ -908,37 +860,34 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>339</v>
+        <v>1080</v>
       </c>
       <c r="E11">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="F11">
-        <v>678</v>
-      </c>
-      <c r="G11" s="2">
-        <v>678</v>
-      </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2560</v>
+      </c>
+      <c r="G11">
+        <v>2160</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="2"/>
-        <v>GOOD!</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.8000000000000002E-2</v>
+        <v>0.018000000000000002</v>
       </c>
       <c r="B12">
         <v>1366</v>
@@ -947,37 +896,34 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>321</v>
+        <v>1080</v>
       </c>
       <c r="E12">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="F12">
-        <v>321</v>
-      </c>
-      <c r="G12" s="2">
-        <v>380</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="0"/>
-        <v>1.1838006230529594</v>
+        <v>2560</v>
+      </c>
+      <c r="G12">
+        <v>1080</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="1"/>
-        <v>1.1838006230529594</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" si="3"/>
-        <v>3.3084112149532698E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="B13">
         <v>360</v>
@@ -986,37 +932,34 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>165</v>
+        <v>320</v>
       </c>
       <c r="E13">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="F13">
-        <v>330</v>
-      </c>
-      <c r="G13" s="2">
-        <v>380</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" si="0"/>
-        <v>2.3030303030303032</v>
+        <v>2560</v>
+      </c>
+      <c r="G13">
+        <v>640</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="1"/>
-        <v>1.1515151515151516</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
-      </c>
-      <c r="K13" s="1">
-        <f t="shared" si="3"/>
-        <v>2.4242424242424255E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="B14">
         <v>768</v>
@@ -1025,37 +968,34 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <v>352</v>
+        <v>728</v>
       </c>
       <c r="E14">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="F14">
-        <v>704</v>
-      </c>
-      <c r="G14" s="2">
-        <v>704</v>
-      </c>
-      <c r="H14" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2560</v>
+      </c>
+      <c r="G14">
+        <v>1456</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="2"/>
-        <v>GOOD!</v>
-      </c>
-      <c r="K14" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.3999999999999999E-2</v>
+        <v>0.013999999999999999</v>
       </c>
       <c r="B15">
         <v>393</v>
@@ -1064,37 +1004,34 @@
         <v>2.75</v>
       </c>
       <c r="D15">
-        <v>180</v>
+        <v>353</v>
       </c>
       <c r="E15">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="F15">
-        <v>360</v>
-      </c>
-      <c r="G15" s="2">
-        <v>380</v>
-      </c>
-      <c r="H15" s="3">
-        <f t="shared" si="0"/>
-        <v>2.1111111111111112</v>
+        <v>2560</v>
+      </c>
+      <c r="G15">
+        <v>706</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I15" s="3">
         <f t="shared" si="1"/>
-        <v>1.0555555555555556</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
-      </c>
-      <c r="K15" s="1">
-        <f t="shared" si="3"/>
-        <v>7.7777777777777806E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.1000000000000001E-2</v>
+        <v>0.011000000000000001</v>
       </c>
       <c r="B16">
         <v>1536</v>
@@ -1103,37 +1040,34 @@
         <v>1.25</v>
       </c>
       <c r="D16">
-        <v>361</v>
+        <v>1080</v>
       </c>
       <c r="E16">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="F16">
-        <v>451</v>
-      </c>
-      <c r="G16" s="2">
-        <v>450</v>
-      </c>
-      <c r="H16" s="3">
-        <f t="shared" si="0"/>
-        <v>1.2465373961218837</v>
+        <v>2560</v>
+      </c>
+      <c r="G16">
+        <v>1350</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I16" s="3">
         <f t="shared" si="1"/>
-        <v>0.99722991689750695</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="2"/>
-        <v>(-)</v>
-      </c>
-      <c r="K16" s="1">
-        <f t="shared" si="3"/>
-        <v>-3.0470914127423535E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="B17">
         <v>320</v>
@@ -1142,50 +1076,47 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>147</v>
+        <v>280</v>
       </c>
       <c r="E17">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="F17">
-        <v>294</v>
-      </c>
-      <c r="G17" s="2">
-        <v>380</v>
-      </c>
-      <c r="H17" s="3">
-        <f t="shared" si="0"/>
-        <v>2.5850340136054424</v>
+        <v>480</v>
+      </c>
+      <c r="G17">
+        <v>560</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="1"/>
-        <v>1.2925170068027212</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="2"/>
-        <v>BIG (++)</v>
-      </c>
-      <c r="K17" s="1">
-        <f t="shared" si="3"/>
-        <v>2.3401360544217696E-3</v>
-      </c>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="2"/>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+      </c>
+      <c r="L17" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>J2="GOOD!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>J2="POOR (--)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>J2="BIG (++)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>OR(J2="(+)",J2="(-)")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>